<commit_message>
Changes in Controller and Pages
</commit_message>
<xml_diff>
--- a/Logbook/WRM Process Log book (1).xlsx
+++ b/Logbook/WRM Process Log book (1).xlsx
@@ -1575,8 +1575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K275"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K90" sqref="K90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>